<commit_message>
Project: LinkedIn Visuals Script: findEmployeeCount Test Status: Completed Feature: Set Data Methods Feature Status: set data methods updated in DataUtil (set int & string data)
</commit_message>
<xml_diff>
--- a/target/test-classes/naukariVisualsData/NaukariVisualsData.xlsx
+++ b/target/test-classes/naukariVisualsData/NaukariVisualsData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Deore\IdeaProjects\ResearchAnalyst\src\test\resources\naukariVisualsData\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>TestCase</t>
   </si>
@@ -163,12 +163,49 @@
   </si>
   <si>
     <t>QTP</t>
+  </si>
+  <si>
+    <t>8838</t>
+  </si>
+  <si>
+    <t>5080</t>
+  </si>
+  <si>
+    <t>1803</t>
+  </si>
+  <si>
+    <t>3705</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>1246</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>6959</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -267,6 +304,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,8 +629,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -608,15 +681,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.88671875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="9.9375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -857,7 +930,9 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -871,7 +946,9 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="19" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -885,7 +962,9 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="20" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -899,7 +978,9 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -913,7 +994,9 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -927,7 +1010,9 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="23" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -941,7 +1026,9 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="24" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -955,7 +1042,9 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="F24" s="25" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -969,7 +1058,9 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="26" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -983,7 +1074,9 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -997,7 +1090,9 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="F27" s="28" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
@@ -1011,7 +1106,9 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="29" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>